<commit_message>
image resizing, html semantics, social media meta tags
</commit_message>
<xml_diff>
--- a/projet4-rapport/Audit_SEO_Lighthouse_Erreurs.xlsx
+++ b/projet4-rapport/Audit_SEO_Lighthouse_Erreurs.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\OpenClassrooms\projet4\Nina-Carducci-Dev\projet4-rapport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50997791-3591-4035-A614-95B2E9841419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -190,8 +196,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,12 +214,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -243,22 +261,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -300,7 +328,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,9 +360,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,6 +412,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,14 +605,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,8 +628,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -576,8 +642,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -590,8 +656,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -604,8 +670,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
@@ -618,8 +684,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
@@ -632,8 +698,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
@@ -646,8 +712,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
@@ -660,8 +726,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
@@ -674,7 +740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -688,7 +754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -702,7 +768,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -716,7 +782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -730,7 +796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -744,7 +810,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -758,7 +824,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -772,7 +838,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -786,7 +852,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -800,7 +866,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -814,7 +880,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -828,7 +894,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -842,7 +908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -856,7 +922,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>

</xml_diff>